<commit_message>
Fetch high point market
</commit_message>
<xml_diff>
--- a/competitors_data_filtered.xlsx
+++ b/competitors_data_filtered.xlsx
@@ -1861,8 +1861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1870,7 +1870,7 @@
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="121.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="181" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="255.6328125" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>